<commit_message>
get_exchange_db.py is now fully functional
Fixed some corner cases, so everything should work now. Had to change
the name of exchange table to exchanges since ‘exchange’ in MySQL is a
special word, and was causing errors when trying to insert values.
</commit_message>
<xml_diff>
--- a/security_master/yahooexchange.xlsx
+++ b/security_master/yahooexchange.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7920" yWindow="-80" windowWidth="25600" windowHeight="14700" tabRatio="500"/>
+    <workbookView xWindow="4420" yWindow="-80" windowWidth="25600" windowHeight="14620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,14 +21,517 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="269">
   <si>
+    <t>Singapore Stock Exchange</t>
+  </si>
+  <si>
+    <t>.SI</t>
+  </si>
+  <si>
+    <t>South Korea</t>
+  </si>
+  <si>
+    <t>Korea Stock Exchange</t>
+  </si>
+  <si>
+    <t>.KS</t>
+  </si>
+  <si>
+    <t>KOSDAQ</t>
+  </si>
+  <si>
+    <t>.KQ</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Barcelona Stock Exchange</t>
+  </si>
+  <si>
+    <t>.BC</t>
+  </si>
+  <si>
+    <t>Bilbao Stock Exchange</t>
+  </si>
+  <si>
+    <t>.BI</t>
+  </si>
+  <si>
+    <t>Madrid Fixed Income Market</t>
+  </si>
+  <si>
+    <t>.MF</t>
+  </si>
+  <si>
+    <t>Madrid Stock Exchange</t>
+  </si>
+  <si>
+    <t>.MA</t>
+  </si>
+  <si>
+    <t>Valencia Stock Exchange</t>
+  </si>
+  <si>
+    <t>.VA</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Stockholm Stock Exchange</t>
+  </si>
+  <si>
+    <t>.ST</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Swiss Exchange</t>
+  </si>
+  <si>
+    <t>.SW</t>
+  </si>
+  <si>
+    <t>Taiwan</t>
+  </si>
+  <si>
+    <t>Taiwan OTC Exchange</t>
+  </si>
+  <si>
+    <t>.TWO</t>
+  </si>
+  <si>
+    <t>Taiwan Stock Exchange</t>
+  </si>
+  <si>
+    <t>.TW</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>Stock Exchange of Thailand (SET)</t>
+  </si>
+  <si>
+    <t>.BK</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Borsa Istanbul</t>
+  </si>
+  <si>
+    <t>.IS</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>FTSE Indices</t>
+  </si>
+  <si>
+    <t>London Stock Exchange</t>
+  </si>
+  <si>
+    <t>.L</t>
+  </si>
+  <si>
+    <t>.IL</t>
+  </si>
+  <si>
+    <t>Venezuela</t>
+  </si>
+  <si>
+    <t>Caracas Stock Exchange</t>
+  </si>
+  <si>
+    <t>.CR</t>
+  </si>
+  <si>
+    <t>Abbreviation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HKG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KSC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KOE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Market, or Index</t>
+  </si>
+  <si>
+    <t>Suffix</t>
+  </si>
+  <si>
+    <t>Delay</t>
+  </si>
+  <si>
+    <t>BIST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FTSE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Toronto Stock Exchange</t>
+  </si>
+  <si>
+    <t>.TO</t>
+  </si>
+  <si>
+    <t>TSX Venture Exchange</t>
+  </si>
+  <si>
+    <t>.V</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>Santiago Stock Exchange</t>
+  </si>
+  <si>
+    <t>.SN</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Shanghai Stock Exchange</t>
+  </si>
+  <si>
+    <t>.SS</t>
+  </si>
+  <si>
+    <t>Shenzhen Stock Exchange</t>
+  </si>
+  <si>
+    <t>.SZ</t>
+  </si>
+  <si>
+    <t>Czech Republic</t>
+  </si>
+  <si>
+    <t>Prague Stock Exchange Index</t>
+  </si>
+  <si>
+    <t>.PR</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Copenhagen Stock Exchange</t>
+  </si>
+  <si>
+    <t>.CO</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>Egyptian Exchange Index</t>
+  </si>
+  <si>
+    <t>.CA</t>
+  </si>
+  <si>
+    <t>Estonia</t>
+  </si>
+  <si>
+    <t>Nasdaq OMX Tallinn</t>
+  </si>
+  <si>
+    <t>.TL</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>Nasdaq OMX Helsinki</t>
+  </si>
+  <si>
+    <t>.HE</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Euronext</t>
+  </si>
+  <si>
+    <t>.NX</t>
+  </si>
+  <si>
+    <t>NYSE Euronext – Paris</t>
+  </si>
+  <si>
+    <t>.PA</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Berlin Stock Exchange</t>
+  </si>
+  <si>
+    <t>.BE</t>
+  </si>
+  <si>
+    <t>Bremen Stock Exchange</t>
+  </si>
+  <si>
+    <t>.BM</t>
+  </si>
+  <si>
+    <t>Dusseldorf Stock Exchange</t>
+  </si>
+  <si>
+    <t>.DU</t>
+  </si>
+  <si>
+    <t>Frankfurt Stock Exchange</t>
+  </si>
+  <si>
+    <t>.F</t>
+  </si>
+  <si>
+    <t>Hamburg Stock Exchange</t>
+  </si>
+  <si>
+    <t>.HM</t>
+  </si>
+  <si>
+    <t>Hanover Stock Exchange</t>
+  </si>
+  <si>
+    <t>.HA</t>
+  </si>
+  <si>
+    <t>Munich Stock Exchange</t>
+  </si>
+  <si>
+    <t>.MU</t>
+  </si>
+  <si>
+    <t>Stuttgart Stock Exchange</t>
+  </si>
+  <si>
+    <t>.SG</t>
+  </si>
+  <si>
+    <t>XETRA Stock Exchange</t>
+  </si>
+  <si>
+    <t>.DE</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>TAI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Athens Stock Exchange</t>
+  </si>
+  <si>
+    <t>.AT</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>Hong Kong Stock Exchange</t>
+  </si>
+  <si>
+    <t>.HK</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>Nasdaq OMX Iceland</t>
+  </si>
+  <si>
+    <t>.IC</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Bombay Stock Exchange</t>
+  </si>
+  <si>
+    <t>.BO</t>
+  </si>
+  <si>
+    <t>National Stock Exchange of India</t>
+  </si>
+  <si>
+    <t>.NS</t>
+  </si>
+  <si>
+    <t>Real-time**</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Jakarta Stock Exchange</t>
+  </si>
+  <si>
+    <t>.JK</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>Irish Stock Exchange</t>
+  </si>
+  <si>
+    <t>.IR</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Tel Aviv Stock Exchange</t>
+  </si>
+  <si>
+    <t>.TA</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>EuroTLX</t>
+  </si>
+  <si>
+    <t>.TI</t>
+  </si>
+  <si>
+    <t>Milan Stock Exchange</t>
+  </si>
+  <si>
+    <t>.MI</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Nikkei Indices</t>
+  </si>
+  <si>
+    <t>Latvia</t>
+  </si>
+  <si>
+    <t>Nasdaq OMX Riga</t>
+  </si>
+  <si>
+    <t>.RG</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Bursa Malaysia</t>
+  </si>
+  <si>
+    <t>.KL</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Mexico Stock Exchange</t>
+  </si>
+  <si>
+    <t>.MX</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>NYSE Euronext – Amsterdam</t>
+  </si>
+  <si>
+    <t>.AS</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>New Zealand Stock Exchange</t>
+  </si>
+  <si>
+    <t>.NZ</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Oslo Stock Exchange</t>
+  </si>
+  <si>
+    <t>.OL</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>NYSE Euronext – Lisbon</t>
+  </si>
+  <si>
+    <t>.LS</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>Qatar Stock Exchange</t>
+  </si>
+  <si>
+    <t>.QA</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Moscow Interbank Currency Exchange (MICEX)</t>
+  </si>
+  <si>
+    <t>.ME</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
     <t>NKY</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FTSE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>AMS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -261,20 +764,16 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Data Provider</t>
+  </si>
+  <si>
+    <t>United States of America</t>
+  </si>
+  <si>
+    <t>BATS Exchange</t>
+  </si>
+  <si>
     <t>N/A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data Provider</t>
-  </si>
-  <si>
-    <t>United States of America</t>
-  </si>
-  <si>
-    <t>BATS Exchange</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
   <si>
     <t>Real-time</t>
@@ -395,505 +894,6 @@
   </si>
   <si>
     <t>Canada</t>
-  </si>
-  <si>
-    <t>Toronto Stock Exchange</t>
-  </si>
-  <si>
-    <t>.TO</t>
-  </si>
-  <si>
-    <t>TSX Venture Exchange</t>
-  </si>
-  <si>
-    <t>.V</t>
-  </si>
-  <si>
-    <t>Chile</t>
-  </si>
-  <si>
-    <t>Santiago Stock Exchange</t>
-  </si>
-  <si>
-    <t>.SN</t>
-  </si>
-  <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>Shanghai Stock Exchange</t>
-  </si>
-  <si>
-    <t>.SS</t>
-  </si>
-  <si>
-    <t>Shenzhen Stock Exchange</t>
-  </si>
-  <si>
-    <t>.SZ</t>
-  </si>
-  <si>
-    <t>Czech Republic</t>
-  </si>
-  <si>
-    <t>Prague Stock Exchange Index</t>
-  </si>
-  <si>
-    <t>.PR</t>
-  </si>
-  <si>
-    <t>Denmark</t>
-  </si>
-  <si>
-    <t>Copenhagen Stock Exchange</t>
-  </si>
-  <si>
-    <t>.CO</t>
-  </si>
-  <si>
-    <t>Egypt</t>
-  </si>
-  <si>
-    <t>Egyptian Exchange Index</t>
-  </si>
-  <si>
-    <t>.CA</t>
-  </si>
-  <si>
-    <t>Estonia</t>
-  </si>
-  <si>
-    <t>Nasdaq OMX Tallinn</t>
-  </si>
-  <si>
-    <t>.TL</t>
-  </si>
-  <si>
-    <t>Finland</t>
-  </si>
-  <si>
-    <t>Nasdaq OMX Helsinki</t>
-  </si>
-  <si>
-    <t>.HE</t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>Euronext</t>
-  </si>
-  <si>
-    <t>.NX</t>
-  </si>
-  <si>
-    <t>NYSE Euronext – Paris</t>
-  </si>
-  <si>
-    <t>.PA</t>
-  </si>
-  <si>
-    <t>Germany</t>
-  </si>
-  <si>
-    <t>Berlin Stock Exchange</t>
-  </si>
-  <si>
-    <t>.BE</t>
-  </si>
-  <si>
-    <t>Bremen Stock Exchange</t>
-  </si>
-  <si>
-    <t>.BM</t>
-  </si>
-  <si>
-    <t>Dusseldorf Stock Exchange</t>
-  </si>
-  <si>
-    <t>.DU</t>
-  </si>
-  <si>
-    <t>Frankfurt Stock Exchange</t>
-  </si>
-  <si>
-    <t>.F</t>
-  </si>
-  <si>
-    <t>Hamburg Stock Exchange</t>
-  </si>
-  <si>
-    <t>.HM</t>
-  </si>
-  <si>
-    <t>Hanover Stock Exchange</t>
-  </si>
-  <si>
-    <t>.HA</t>
-  </si>
-  <si>
-    <t>Munich Stock Exchange</t>
-  </si>
-  <si>
-    <t>.MU</t>
-  </si>
-  <si>
-    <t>Stuttgart Stock Exchange</t>
-  </si>
-  <si>
-    <t>.SG</t>
-  </si>
-  <si>
-    <t>XETRA Stock Exchange</t>
-  </si>
-  <si>
-    <t>.DE</t>
-  </si>
-  <si>
-    <t>Greece</t>
-  </si>
-  <si>
-    <t>TAI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GER</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>STU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Athens Stock Exchange</t>
-  </si>
-  <si>
-    <t>.AT</t>
-  </si>
-  <si>
-    <t>Hong Kong</t>
-  </si>
-  <si>
-    <t>Hong Kong Stock Exchange</t>
-  </si>
-  <si>
-    <t>.HK</t>
-  </si>
-  <si>
-    <t>Iceland</t>
-  </si>
-  <si>
-    <t>Nasdaq OMX Iceland</t>
-  </si>
-  <si>
-    <t>.IC</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>Bombay Stock Exchange</t>
-  </si>
-  <si>
-    <t>.BO</t>
-  </si>
-  <si>
-    <t>National Stock Exchange of India</t>
-  </si>
-  <si>
-    <t>.NS</t>
-  </si>
-  <si>
-    <t>Real-time**</t>
-  </si>
-  <si>
-    <t>Indonesia</t>
-  </si>
-  <si>
-    <t>Jakarta Stock Exchange</t>
-  </si>
-  <si>
-    <t>.JK</t>
-  </si>
-  <si>
-    <t>Ireland</t>
-  </si>
-  <si>
-    <t>Irish Stock Exchange</t>
-  </si>
-  <si>
-    <t>.IR</t>
-  </si>
-  <si>
-    <t>Israel</t>
-  </si>
-  <si>
-    <t>Tel Aviv Stock Exchange</t>
-  </si>
-  <si>
-    <t>.TA</t>
-  </si>
-  <si>
-    <t>Italy</t>
-  </si>
-  <si>
-    <t>EuroTLX</t>
-  </si>
-  <si>
-    <t>.TI</t>
-  </si>
-  <si>
-    <t>Milan Stock Exchange</t>
-  </si>
-  <si>
-    <t>.MI</t>
-  </si>
-  <si>
-    <t>Japan</t>
-  </si>
-  <si>
-    <t>Nikkei Indices</t>
-  </si>
-  <si>
-    <t>Latvia</t>
-  </si>
-  <si>
-    <t>Nasdaq OMX Riga</t>
-  </si>
-  <si>
-    <t>.RG</t>
-  </si>
-  <si>
-    <t>Malaysia</t>
-  </si>
-  <si>
-    <t>Bursa Malaysia</t>
-  </si>
-  <si>
-    <t>.KL</t>
-  </si>
-  <si>
-    <t>Mexico</t>
-  </si>
-  <si>
-    <t>Mexico Stock Exchange</t>
-  </si>
-  <si>
-    <t>.MX</t>
-  </si>
-  <si>
-    <t>Netherlands</t>
-  </si>
-  <si>
-    <t>NYSE Euronext – Amsterdam</t>
-  </si>
-  <si>
-    <t>.AS</t>
-  </si>
-  <si>
-    <t>New Zealand</t>
-  </si>
-  <si>
-    <t>New Zealand Stock Exchange</t>
-  </si>
-  <si>
-    <t>.NZ</t>
-  </si>
-  <si>
-    <t>Norway</t>
-  </si>
-  <si>
-    <t>Oslo Stock Exchange</t>
-  </si>
-  <si>
-    <t>.OL</t>
-  </si>
-  <si>
-    <t>Portugal</t>
-  </si>
-  <si>
-    <t>NYSE Euronext – Lisbon</t>
-  </si>
-  <si>
-    <t>.LS</t>
-  </si>
-  <si>
-    <t>Qatar</t>
-  </si>
-  <si>
-    <t>Qatar Stock Exchange</t>
-  </si>
-  <si>
-    <t>.QA</t>
-  </si>
-  <si>
-    <t>Russia</t>
-  </si>
-  <si>
-    <t>Moscow Interbank Currency Exchange (MICEX)</t>
-  </si>
-  <si>
-    <t>.ME</t>
-  </si>
-  <si>
-    <t>Singapore</t>
-  </si>
-  <si>
-    <t>Singapore Stock Exchange</t>
-  </si>
-  <si>
-    <t>.SI</t>
-  </si>
-  <si>
-    <t>South Korea</t>
-  </si>
-  <si>
-    <t>Korea Stock Exchange</t>
-  </si>
-  <si>
-    <t>.KS</t>
-  </si>
-  <si>
-    <t>KOSDAQ</t>
-  </si>
-  <si>
-    <t>.KQ</t>
-  </si>
-  <si>
-    <t>Spain</t>
-  </si>
-  <si>
-    <t>Barcelona Stock Exchange</t>
-  </si>
-  <si>
-    <t>.BC</t>
-  </si>
-  <si>
-    <t>Bilbao Stock Exchange</t>
-  </si>
-  <si>
-    <t>.BI</t>
-  </si>
-  <si>
-    <t>Madrid Fixed Income Market</t>
-  </si>
-  <si>
-    <t>.MF</t>
-  </si>
-  <si>
-    <t>Madrid Stock Exchange</t>
-  </si>
-  <si>
-    <t>.MA</t>
-  </si>
-  <si>
-    <t>Valencia Stock Exchange</t>
-  </si>
-  <si>
-    <t>.VA</t>
-  </si>
-  <si>
-    <t>Sweden</t>
-  </si>
-  <si>
-    <t>Stockholm Stock Exchange</t>
-  </si>
-  <si>
-    <t>.ST</t>
-  </si>
-  <si>
-    <t>Switzerland</t>
-  </si>
-  <si>
-    <t>Swiss Exchange</t>
-  </si>
-  <si>
-    <t>.SW</t>
-  </si>
-  <si>
-    <t>Taiwan</t>
-  </si>
-  <si>
-    <t>Taiwan OTC Exchange</t>
-  </si>
-  <si>
-    <t>.TWO</t>
-  </si>
-  <si>
-    <t>Taiwan Stock Exchange</t>
-  </si>
-  <si>
-    <t>.TW</t>
-  </si>
-  <si>
-    <t>Thailand</t>
-  </si>
-  <si>
-    <t>Stock Exchange of Thailand (SET)</t>
-  </si>
-  <si>
-    <t>.BK</t>
-  </si>
-  <si>
-    <t>Turkey</t>
-  </si>
-  <si>
-    <t>Borsa Istanbul</t>
-  </si>
-  <si>
-    <t>.IS</t>
-  </si>
-  <si>
-    <t>United Kingdom</t>
-  </si>
-  <si>
-    <t>FTSE Indices</t>
-  </si>
-  <si>
-    <t>London Stock Exchange</t>
-  </si>
-  <si>
-    <t>.L</t>
-  </si>
-  <si>
-    <t>.IL</t>
-  </si>
-  <si>
-    <t>Venezuela</t>
-  </si>
-  <si>
-    <t>Caracas Stock Exchange</t>
-  </si>
-  <si>
-    <t>.CR</t>
-  </si>
-  <si>
-    <t>Abbreviation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HKG</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>KSC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>KOE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Market, or Index</t>
-  </si>
-  <si>
-    <t>Suffix</t>
-  </si>
-  <si>
-    <t>Delay</t>
   </si>
 </sst>
 </file>
@@ -1268,8 +1268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:F77"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1281,1518 +1281,1518 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>265</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>266</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
-        <v>267</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>268</v>
+        <v>50</v>
       </c>
       <c r="E1" t="s">
-        <v>61</v>
+        <v>225</v>
       </c>
       <c r="F1" t="s">
-        <v>261</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>226</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>227</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>228</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>226</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>231</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>232</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>233</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>226</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>235</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>236</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>233</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>226</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>237</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>228</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>226</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>238</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>228</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="E6" t="s">
-        <v>66</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>226</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>239</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>240</v>
       </c>
       <c r="D7" t="s">
-        <v>77</v>
+        <v>241</v>
       </c>
       <c r="E7" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>226</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>242</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>243</v>
       </c>
       <c r="D8" t="s">
-        <v>77</v>
+        <v>241</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>226</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>244</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>228</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="E9" t="s">
-        <v>81</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>226</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>246</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>228</v>
       </c>
       <c r="D10" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E10" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>226</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>248</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>228</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="E11" t="s">
-        <v>66</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>226</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>249</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>228</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>226</v>
       </c>
       <c r="B13" t="s">
-        <v>86</v>
+        <v>250</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>228</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>251</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>252</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>253</v>
       </c>
       <c r="D14" t="s">
-        <v>77</v>
+        <v>241</v>
       </c>
       <c r="E14" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F14" t="s">
-        <v>22</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>254</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>255</v>
       </c>
       <c r="C15" t="s">
-        <v>92</v>
+        <v>256</v>
       </c>
       <c r="D15" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E15" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F15" t="s">
-        <v>16</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>94</v>
+        <v>258</v>
       </c>
       <c r="B16" t="s">
-        <v>95</v>
+        <v>259</v>
       </c>
       <c r="C16" t="s">
-        <v>96</v>
+        <v>260</v>
       </c>
       <c r="D16" t="s">
-        <v>97</v>
+        <v>261</v>
       </c>
       <c r="E16" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F16" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>98</v>
+        <v>262</v>
       </c>
       <c r="B17" t="s">
-        <v>99</v>
+        <v>263</v>
       </c>
       <c r="C17" t="s">
-        <v>100</v>
+        <v>264</v>
       </c>
       <c r="D17" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E17" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F17" t="s">
-        <v>24</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>265</v>
       </c>
       <c r="B18" t="s">
-        <v>102</v>
+        <v>266</v>
       </c>
       <c r="C18" t="s">
-        <v>103</v>
+        <v>267</v>
       </c>
       <c r="D18" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E18" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F18" t="s">
-        <v>55</v>
+        <v>220</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>268</v>
       </c>
       <c r="B19" t="s">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>106</v>
+        <v>54</v>
       </c>
       <c r="D19" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E19" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F19" t="s">
-        <v>25</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>104</v>
+        <v>268</v>
       </c>
       <c r="B20" t="s">
-        <v>107</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="D20" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E20" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F20" t="s">
-        <v>26</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>109</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>110</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>111</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E21" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F21" t="s">
-        <v>27</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>112</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>113</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>114</v>
+        <v>62</v>
       </c>
       <c r="D22" t="s">
-        <v>77</v>
+        <v>241</v>
       </c>
       <c r="E22" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F22" t="s">
-        <v>17</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>112</v>
+        <v>60</v>
       </c>
       <c r="B23" t="s">
-        <v>115</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s">
-        <v>116</v>
+        <v>64</v>
       </c>
       <c r="D23" t="s">
-        <v>77</v>
+        <v>241</v>
       </c>
       <c r="E23" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F23" t="s">
-        <v>28</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>117</v>
+        <v>65</v>
       </c>
       <c r="B24" t="s">
-        <v>118</v>
+        <v>66</v>
       </c>
       <c r="C24" t="s">
-        <v>119</v>
+        <v>67</v>
       </c>
       <c r="D24" t="s">
-        <v>97</v>
+        <v>261</v>
       </c>
       <c r="E24" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F24" t="s">
-        <v>29</v>
+        <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>120</v>
+        <v>68</v>
       </c>
       <c r="B25" t="s">
-        <v>121</v>
+        <v>69</v>
       </c>
       <c r="C25" t="s">
-        <v>122</v>
+        <v>70</v>
       </c>
       <c r="D25" t="s">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="E25" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F25" t="s">
-        <v>30</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>123</v>
+        <v>71</v>
       </c>
       <c r="B26" t="s">
-        <v>124</v>
+        <v>72</v>
       </c>
       <c r="C26" t="s">
-        <v>125</v>
+        <v>73</v>
       </c>
       <c r="D26" t="s">
-        <v>97</v>
+        <v>261</v>
       </c>
       <c r="E26" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F26" t="s">
-        <v>5</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>126</v>
+        <v>74</v>
       </c>
       <c r="B27" t="s">
-        <v>127</v>
+        <v>75</v>
       </c>
       <c r="C27" t="s">
-        <v>128</v>
+        <v>76</v>
       </c>
       <c r="D27" t="s">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="E27" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F27" t="s">
-        <v>31</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>129</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
-        <v>130</v>
+        <v>78</v>
       </c>
       <c r="C28" t="s">
-        <v>131</v>
+        <v>79</v>
       </c>
       <c r="D28" t="s">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="E28" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F28" t="s">
-        <v>32</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>132</v>
+        <v>80</v>
       </c>
       <c r="B29" t="s">
-        <v>133</v>
+        <v>81</v>
       </c>
       <c r="C29" t="s">
-        <v>134</v>
+        <v>82</v>
       </c>
       <c r="D29" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E29" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F29" t="s">
-        <v>33</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>132</v>
+        <v>80</v>
       </c>
       <c r="B30" t="s">
-        <v>135</v>
+        <v>83</v>
       </c>
       <c r="C30" t="s">
-        <v>136</v>
+        <v>84</v>
       </c>
       <c r="D30" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E30" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F30" t="s">
-        <v>57</v>
+        <v>222</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>137</v>
+        <v>85</v>
       </c>
       <c r="B31" t="s">
-        <v>138</v>
+        <v>86</v>
       </c>
       <c r="C31" t="s">
-        <v>139</v>
+        <v>87</v>
       </c>
       <c r="D31" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E31" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F31" t="s">
-        <v>56</v>
+        <v>221</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>137</v>
+        <v>85</v>
       </c>
       <c r="B32" t="s">
-        <v>140</v>
+        <v>88</v>
       </c>
       <c r="C32" t="s">
-        <v>141</v>
+        <v>89</v>
       </c>
       <c r="D32" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E32" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F32" t="s">
-        <v>34</v>
+        <v>199</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>137</v>
+        <v>85</v>
       </c>
       <c r="B33" t="s">
-        <v>142</v>
+        <v>90</v>
       </c>
       <c r="C33" t="s">
-        <v>143</v>
+        <v>91</v>
       </c>
       <c r="D33" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E33" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F33" t="s">
-        <v>8</v>
+        <v>173</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>137</v>
+        <v>85</v>
       </c>
       <c r="B34" t="s">
-        <v>144</v>
+        <v>92</v>
       </c>
       <c r="C34" t="s">
-        <v>145</v>
+        <v>93</v>
       </c>
       <c r="D34" t="s">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="E34" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F34" t="s">
-        <v>158</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>137</v>
+        <v>85</v>
       </c>
       <c r="B35" t="s">
-        <v>146</v>
+        <v>94</v>
       </c>
       <c r="C35" t="s">
-        <v>147</v>
+        <v>95</v>
       </c>
       <c r="D35" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E35" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F35" t="s">
-        <v>9</v>
+        <v>174</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>137</v>
+        <v>85</v>
       </c>
       <c r="B36" t="s">
-        <v>148</v>
+        <v>96</v>
       </c>
       <c r="C36" t="s">
-        <v>149</v>
+        <v>97</v>
       </c>
       <c r="D36" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E36" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F36" t="s">
-        <v>12</v>
+        <v>177</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>137</v>
+        <v>85</v>
       </c>
       <c r="B37" t="s">
-        <v>150</v>
+        <v>98</v>
       </c>
       <c r="C37" t="s">
-        <v>151</v>
+        <v>99</v>
       </c>
       <c r="D37" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E37" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F37" t="s">
-        <v>10</v>
+        <v>175</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>137</v>
+        <v>85</v>
       </c>
       <c r="B38" t="s">
-        <v>152</v>
+        <v>100</v>
       </c>
       <c r="C38" t="s">
-        <v>153</v>
+        <v>101</v>
       </c>
       <c r="D38" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E38" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F38" t="s">
-        <v>159</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>137</v>
+        <v>85</v>
       </c>
       <c r="B39" t="s">
-        <v>154</v>
+        <v>102</v>
       </c>
       <c r="C39" t="s">
-        <v>155</v>
+        <v>103</v>
       </c>
       <c r="D39" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E39" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F39" t="s">
-        <v>158</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>156</v>
+        <v>104</v>
       </c>
       <c r="B40" t="s">
-        <v>160</v>
+        <v>108</v>
       </c>
       <c r="C40" t="s">
-        <v>161</v>
+        <v>109</v>
       </c>
       <c r="D40" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E40" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F40" t="s">
-        <v>35</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>162</v>
+        <v>110</v>
       </c>
       <c r="B41" t="s">
-        <v>163</v>
+        <v>111</v>
       </c>
       <c r="C41" t="s">
-        <v>164</v>
+        <v>112</v>
       </c>
       <c r="D41" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E41" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F41" t="s">
-        <v>262</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>165</v>
+        <v>113</v>
       </c>
       <c r="B42" t="s">
-        <v>166</v>
+        <v>114</v>
       </c>
       <c r="C42" t="s">
-        <v>167</v>
+        <v>115</v>
       </c>
       <c r="D42" t="s">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="E42" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F42" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>168</v>
+        <v>116</v>
       </c>
       <c r="B43" t="s">
-        <v>169</v>
+        <v>117</v>
       </c>
       <c r="C43" t="s">
-        <v>170</v>
+        <v>118</v>
       </c>
       <c r="D43" t="s">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="E43" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F43" t="s">
-        <v>36</v>
+        <v>201</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>168</v>
+        <v>116</v>
       </c>
       <c r="B44" t="s">
-        <v>171</v>
+        <v>119</v>
       </c>
       <c r="C44" t="s">
-        <v>172</v>
+        <v>120</v>
       </c>
       <c r="D44" t="s">
-        <v>173</v>
+        <v>121</v>
       </c>
       <c r="E44" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F44" t="s">
-        <v>37</v>
+        <v>202</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>174</v>
+        <v>122</v>
       </c>
       <c r="B45" t="s">
-        <v>175</v>
+        <v>123</v>
       </c>
       <c r="C45" t="s">
-        <v>176</v>
+        <v>124</v>
       </c>
       <c r="D45" t="s">
-        <v>69</v>
+        <v>233</v>
       </c>
       <c r="E45" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F45" t="s">
-        <v>38</v>
+        <v>203</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>177</v>
+        <v>125</v>
       </c>
       <c r="B46" t="s">
-        <v>178</v>
+        <v>126</v>
       </c>
       <c r="C46" t="s">
-        <v>179</v>
+        <v>127</v>
       </c>
       <c r="D46" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E46" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F46" t="s">
-        <v>39</v>
+        <v>204</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>180</v>
+        <v>128</v>
       </c>
       <c r="B47" t="s">
-        <v>181</v>
+        <v>129</v>
       </c>
       <c r="C47" t="s">
-        <v>182</v>
+        <v>130</v>
       </c>
       <c r="D47" t="s">
-        <v>97</v>
+        <v>261</v>
       </c>
       <c r="E47" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F47" t="s">
-        <v>58</v>
+        <v>223</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>183</v>
+        <v>131</v>
       </c>
       <c r="B48" t="s">
-        <v>184</v>
+        <v>132</v>
       </c>
       <c r="C48" t="s">
-        <v>185</v>
+        <v>133</v>
       </c>
       <c r="D48" t="s">
-        <v>97</v>
+        <v>261</v>
       </c>
       <c r="E48" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F48" t="s">
-        <v>59</v>
+        <v>224</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>183</v>
+        <v>131</v>
       </c>
       <c r="B49" t="s">
-        <v>186</v>
+        <v>134</v>
       </c>
       <c r="C49" t="s">
-        <v>187</v>
+        <v>135</v>
       </c>
       <c r="D49" t="s">
-        <v>97</v>
+        <v>261</v>
       </c>
       <c r="E49" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F49" t="s">
-        <v>40</v>
+        <v>205</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>188</v>
+        <v>136</v>
       </c>
       <c r="B50" t="s">
-        <v>189</v>
+        <v>137</v>
       </c>
       <c r="C50" t="s">
-        <v>64</v>
+        <v>228</v>
       </c>
       <c r="D50" t="s">
-        <v>77</v>
+        <v>241</v>
       </c>
       <c r="E50" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F50" t="s">
-        <v>0</v>
+        <v>166</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>190</v>
+        <v>138</v>
       </c>
       <c r="B51" t="s">
-        <v>191</v>
+        <v>139</v>
       </c>
       <c r="C51" t="s">
-        <v>192</v>
+        <v>140</v>
       </c>
       <c r="D51" t="s">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="E51" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F51" t="s">
-        <v>3</v>
+        <v>168</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>193</v>
+        <v>141</v>
       </c>
       <c r="B52" t="s">
-        <v>194</v>
+        <v>142</v>
       </c>
       <c r="C52" t="s">
-        <v>195</v>
+        <v>143</v>
       </c>
       <c r="D52" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E52" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F52" t="s">
-        <v>53</v>
+        <v>218</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>196</v>
+        <v>144</v>
       </c>
       <c r="B53" t="s">
-        <v>197</v>
+        <v>145</v>
       </c>
       <c r="C53" t="s">
-        <v>198</v>
+        <v>146</v>
       </c>
       <c r="D53" t="s">
-        <v>97</v>
+        <v>261</v>
       </c>
       <c r="E53" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F53" t="s">
-        <v>54</v>
+        <v>219</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>199</v>
+        <v>147</v>
       </c>
       <c r="B54" t="s">
-        <v>200</v>
+        <v>148</v>
       </c>
       <c r="C54" t="s">
-        <v>201</v>
+        <v>149</v>
       </c>
       <c r="D54" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E54" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F54" t="s">
-        <v>2</v>
+        <v>167</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>202</v>
+        <v>150</v>
       </c>
       <c r="B55" t="s">
-        <v>203</v>
+        <v>151</v>
       </c>
       <c r="C55" t="s">
-        <v>204</v>
+        <v>152</v>
       </c>
       <c r="D55" t="s">
-        <v>97</v>
+        <v>261</v>
       </c>
       <c r="E55" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F55" t="s">
-        <v>41</v>
+        <v>206</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>205</v>
+        <v>153</v>
       </c>
       <c r="B56" t="s">
-        <v>206</v>
+        <v>154</v>
       </c>
       <c r="C56" t="s">
+        <v>155</v>
+      </c>
+      <c r="D56" t="s">
+        <v>247</v>
+      </c>
+      <c r="E56" t="s">
+        <v>257</v>
+      </c>
+      <c r="F56" t="s">
         <v>207</v>
-      </c>
-      <c r="D56" t="s">
-        <v>83</v>
-      </c>
-      <c r="E56" t="s">
-        <v>93</v>
-      </c>
-      <c r="F56" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
+        <v>156</v>
+      </c>
+      <c r="B57" t="s">
+        <v>157</v>
+      </c>
+      <c r="C57" t="s">
+        <v>158</v>
+      </c>
+      <c r="D57" t="s">
+        <v>247</v>
+      </c>
+      <c r="E57" t="s">
+        <v>257</v>
+      </c>
+      <c r="F57" t="s">
         <v>208</v>
-      </c>
-      <c r="B57" t="s">
-        <v>209</v>
-      </c>
-      <c r="C57" t="s">
-        <v>210</v>
-      </c>
-      <c r="D57" t="s">
-        <v>83</v>
-      </c>
-      <c r="E57" t="s">
-        <v>93</v>
-      </c>
-      <c r="F57" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>211</v>
+        <v>159</v>
       </c>
       <c r="B58" t="s">
-        <v>212</v>
+        <v>160</v>
       </c>
       <c r="C58" t="s">
-        <v>213</v>
+        <v>161</v>
       </c>
       <c r="D58" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E58" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F58" t="s">
-        <v>7</v>
+        <v>172</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>214</v>
+        <v>162</v>
       </c>
       <c r="B59" t="s">
-        <v>215</v>
+        <v>163</v>
       </c>
       <c r="C59" t="s">
-        <v>216</v>
+        <v>164</v>
       </c>
       <c r="D59" t="s">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="E59" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F59" t="s">
-        <v>44</v>
+        <v>209</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>217</v>
+        <v>165</v>
       </c>
       <c r="B60" t="s">
-        <v>218</v>
+        <v>0</v>
       </c>
       <c r="C60" t="s">
-        <v>219</v>
+        <v>1</v>
       </c>
       <c r="D60" t="s">
-        <v>97</v>
+        <v>261</v>
       </c>
       <c r="E60" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F60" t="s">
-        <v>6</v>
+        <v>171</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>220</v>
+        <v>2</v>
       </c>
       <c r="B61" t="s">
-        <v>221</v>
+        <v>3</v>
       </c>
       <c r="C61" t="s">
-        <v>222</v>
+        <v>4</v>
       </c>
       <c r="D61" t="s">
-        <v>97</v>
+        <v>261</v>
       </c>
       <c r="E61" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F61" t="s">
-        <v>263</v>
+        <v>45</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>220</v>
+        <v>2</v>
       </c>
       <c r="B62" t="s">
-        <v>223</v>
+        <v>5</v>
       </c>
       <c r="C62" t="s">
-        <v>224</v>
+        <v>6</v>
       </c>
       <c r="D62" t="s">
-        <v>97</v>
+        <v>261</v>
       </c>
       <c r="E62" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F62" t="s">
-        <v>264</v>
+        <v>46</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>225</v>
+        <v>7</v>
       </c>
       <c r="B63" t="s">
-        <v>226</v>
+        <v>8</v>
       </c>
       <c r="C63" t="s">
-        <v>227</v>
+        <v>9</v>
       </c>
       <c r="D63" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E63" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F63" t="s">
-        <v>45</v>
+        <v>210</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>225</v>
+        <v>7</v>
       </c>
       <c r="B64" t="s">
-        <v>228</v>
+        <v>10</v>
       </c>
       <c r="C64" t="s">
-        <v>229</v>
+        <v>11</v>
       </c>
       <c r="D64" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E64" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F64" t="s">
-        <v>46</v>
+        <v>211</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>225</v>
+        <v>7</v>
       </c>
       <c r="B65" t="s">
-        <v>230</v>
+        <v>12</v>
       </c>
       <c r="C65" t="s">
-        <v>231</v>
+        <v>13</v>
       </c>
       <c r="D65" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E65" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F65" t="s">
-        <v>47</v>
+        <v>212</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>225</v>
+        <v>7</v>
       </c>
       <c r="B66" t="s">
-        <v>232</v>
+        <v>14</v>
       </c>
       <c r="C66" t="s">
-        <v>233</v>
+        <v>15</v>
       </c>
       <c r="D66" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E66" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F66" t="s">
-        <v>14</v>
+        <v>179</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>225</v>
+        <v>7</v>
       </c>
       <c r="B67" t="s">
-        <v>234</v>
+        <v>16</v>
       </c>
       <c r="C67" t="s">
-        <v>235</v>
+        <v>17</v>
       </c>
       <c r="D67" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E67" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F67" t="s">
-        <v>48</v>
+        <v>213</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>236</v>
+        <v>18</v>
       </c>
       <c r="B68" t="s">
-        <v>237</v>
+        <v>19</v>
       </c>
       <c r="C68" t="s">
-        <v>238</v>
+        <v>20</v>
       </c>
       <c r="D68" t="s">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="E68" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F68" t="s">
-        <v>52</v>
+        <v>217</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>239</v>
+        <v>21</v>
       </c>
       <c r="B69" t="s">
-        <v>240</v>
+        <v>22</v>
       </c>
       <c r="C69" t="s">
+        <v>23</v>
+      </c>
+      <c r="D69" t="s">
         <v>241</v>
       </c>
-      <c r="D69" t="s">
-        <v>77</v>
-      </c>
       <c r="E69" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F69" t="s">
-        <v>49</v>
+        <v>214</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>242</v>
+        <v>24</v>
       </c>
       <c r="B70" t="s">
-        <v>243</v>
+        <v>25</v>
       </c>
       <c r="C70" t="s">
-        <v>244</v>
+        <v>26</v>
       </c>
       <c r="D70" t="s">
-        <v>97</v>
+        <v>261</v>
       </c>
       <c r="E70" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F70" t="s">
-        <v>13</v>
+        <v>178</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>242</v>
+        <v>24</v>
       </c>
       <c r="B71" t="s">
-        <v>245</v>
+        <v>27</v>
       </c>
       <c r="C71" t="s">
-        <v>246</v>
+        <v>28</v>
       </c>
       <c r="D71" t="s">
-        <v>97</v>
+        <v>261</v>
       </c>
       <c r="E71" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F71" t="s">
-        <v>157</v>
+        <v>105</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>247</v>
+        <v>29</v>
       </c>
       <c r="B72" t="s">
-        <v>248</v>
+        <v>30</v>
       </c>
       <c r="C72" t="s">
-        <v>249</v>
+        <v>31</v>
       </c>
       <c r="D72" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E72" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F72" t="s">
-        <v>50</v>
+        <v>215</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>250</v>
+        <v>32</v>
       </c>
       <c r="B73" t="s">
-        <v>251</v>
+        <v>33</v>
       </c>
       <c r="C73" t="s">
-        <v>252</v>
+        <v>34</v>
       </c>
       <c r="D73" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E73" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F73" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>253</v>
+        <v>35</v>
       </c>
       <c r="B74" t="s">
-        <v>254</v>
+        <v>36</v>
       </c>
       <c r="C74" t="s">
-        <v>64</v>
+        <v>228</v>
       </c>
       <c r="D74" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E74" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F74" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>253</v>
+        <v>35</v>
       </c>
       <c r="B75" t="s">
-        <v>255</v>
+        <v>37</v>
       </c>
       <c r="C75" t="s">
-        <v>256</v>
+        <v>38</v>
       </c>
       <c r="D75" t="s">
-        <v>97</v>
+        <v>261</v>
       </c>
       <c r="E75" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F75" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>253</v>
+        <v>35</v>
       </c>
       <c r="B76" t="s">
-        <v>255</v>
+        <v>37</v>
       </c>
       <c r="C76" t="s">
-        <v>257</v>
+        <v>39</v>
       </c>
       <c r="D76" t="s">
-        <v>97</v>
+        <v>261</v>
       </c>
       <c r="E76" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="F76" t="s">
-        <v>15</v>
+        <v>180</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>258</v>
+        <v>40</v>
       </c>
       <c r="B77" t="s">
-        <v>259</v>
+        <v>41</v>
       </c>
       <c r="C77" t="s">
-        <v>260</v>
+        <v>42</v>
       </c>
       <c r="D77" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="E77" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="F77" t="s">
-        <v>51</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated get_exchange_db.py and insert_symbol_db.py
insert_symbol_db.py now gets the exchanged from the exchanges table,
linking them together
</commit_message>
<xml_diff>
--- a/security_master/yahooexchange.xlsx
+++ b/security_master/yahooexchange.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="-80" windowWidth="25600" windowHeight="14620" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="14440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,580 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="277">
+  <si>
+    <t>TLO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data Provider</t>
+  </si>
+  <si>
+    <t>United States of America</t>
+  </si>
+  <si>
+    <t>BATS Exchange</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Real-time</t>
+  </si>
+  <si>
+    <t>Direct from Exchange</t>
+  </si>
+  <si>
+    <t>Chicago Board of Trade</t>
+  </si>
+  <si>
+    <t>.CBT</t>
+  </si>
+  <si>
+    <t>10 min</t>
+  </si>
+  <si>
+    <t>Interactive Data Real-Time Services</t>
+  </si>
+  <si>
+    <t>Chicago Mercantile Exchange</t>
+  </si>
+  <si>
+    <t>.CME</t>
+  </si>
+  <si>
+    <t>Dow Jones Indexes</t>
+  </si>
+  <si>
+    <t>NASDAQ Stock Exchange</t>
+  </si>
+  <si>
+    <t>New York Board of Trade</t>
+  </si>
+  <si>
+    <t>.NYB</t>
+  </si>
+  <si>
+    <t>30 min</t>
+  </si>
+  <si>
+    <t>New York Mercantile Exchange</t>
+  </si>
+  <si>
+    <t>.NYM</t>
+  </si>
+  <si>
+    <t>New York Stock Exchange</t>
+  </si>
+  <si>
+    <t>Direct from Exchange***</t>
+  </si>
+  <si>
+    <t>OPRA</t>
+  </si>
+  <si>
+    <t>15 min</t>
+  </si>
+  <si>
+    <t>OTC Bulletin Board Market</t>
+  </si>
+  <si>
+    <t>OTC Markets Group</t>
+  </si>
+  <si>
+    <t>S &amp; P Indices</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Buenos Aires Stock Exchange</t>
+  </si>
+  <si>
+    <t>.BA</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Vienna Stock Exchange</t>
+  </si>
+  <si>
+    <t>.VI</t>
+  </si>
+  <si>
+    <t>SIX Financial Information</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Australian Stock Exchange</t>
+  </si>
+  <si>
+    <t>.AX</t>
+  </si>
+  <si>
+    <t>20 min</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>NYSE Euronext - Brussels</t>
+  </si>
+  <si>
+    <t>.BR</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>BOVESPA - Sao Paolo Stock Exchange</t>
+  </si>
+  <si>
+    <t>.SA</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>NYSE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OTC BB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NasdaqGS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>London Stock Exchange (L)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>London Stock Exchange (IL)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NSE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TSXV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HKSE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Other OTC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OOTC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>World</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NZSE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hong Kong Stock Exchange</t>
+  </si>
+  <si>
+    <t>.HK</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>Nasdaq OMX Iceland</t>
+  </si>
+  <si>
+    <t>.IC</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Bombay Stock Exchange</t>
+  </si>
+  <si>
+    <t>.BO</t>
+  </si>
+  <si>
+    <t>National Stock Exchange of India</t>
+  </si>
+  <si>
+    <t>.NS</t>
+  </si>
+  <si>
+    <t>Real-time**</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Jakarta Stock Exchange</t>
+  </si>
+  <si>
+    <t>.JK</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>Irish Stock Exchange</t>
+  </si>
+  <si>
+    <t>.IR</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Tel Aviv Stock Exchange</t>
+  </si>
+  <si>
+    <t>.TA</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>EuroTLX</t>
+  </si>
+  <si>
+    <t>.TI</t>
+  </si>
+  <si>
+    <t>Milan Stock Exchange</t>
+  </si>
+  <si>
+    <t>.MI</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Nikkei Indices</t>
+  </si>
+  <si>
+    <t>Latvia</t>
+  </si>
+  <si>
+    <t>Nasdaq OMX Riga</t>
+  </si>
+  <si>
+    <t>.RG</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Bursa Malaysia</t>
+  </si>
+  <si>
+    <t>.KL</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Mexico Stock Exchange</t>
+  </si>
+  <si>
+    <t>.MX</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>NYSE Euronext – Amsterdam</t>
+  </si>
+  <si>
+    <t>.AS</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>New Zealand Stock Exchange</t>
+  </si>
+  <si>
+    <t>.NZ</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Oslo Stock Exchange</t>
+  </si>
+  <si>
+    <t>.OL</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>NYSE Euronext – Lisbon</t>
+  </si>
+  <si>
+    <t>.LS</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>Qatar Stock Exchange</t>
+  </si>
+  <si>
+    <t>.QA</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Moscow Interbank Currency Exchange (MICEX)</t>
+  </si>
+  <si>
+    <t>.ME</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>NKY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RIX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ICX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EGX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SES</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QSE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DUS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FRA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MUN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LSE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HAM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TWO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IOB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VIE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CBT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NBI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NYM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BUE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BRU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TOR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SGO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TLX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HEL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BRE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BSE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JKT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MIL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OSL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LIS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MCX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BAR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BIL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MFI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VAL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SWX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KLS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MEX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SAO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TLV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>Singapore Stock Exchange</t>
   </si>
@@ -132,9 +705,6 @@
     <t>FTSE Indices</t>
   </si>
   <si>
-    <t>London Stock Exchange</t>
-  </si>
-  <si>
     <t>.L</t>
   </si>
   <si>
@@ -154,10 +724,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>HKG</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>KSC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -361,539 +927,6 @@
   </si>
   <si>
     <t>Hong Kong</t>
-  </si>
-  <si>
-    <t>Hong Kong Stock Exchange</t>
-  </si>
-  <si>
-    <t>.HK</t>
-  </si>
-  <si>
-    <t>Iceland</t>
-  </si>
-  <si>
-    <t>Nasdaq OMX Iceland</t>
-  </si>
-  <si>
-    <t>.IC</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>Bombay Stock Exchange</t>
-  </si>
-  <si>
-    <t>.BO</t>
-  </si>
-  <si>
-    <t>National Stock Exchange of India</t>
-  </si>
-  <si>
-    <t>.NS</t>
-  </si>
-  <si>
-    <t>Real-time**</t>
-  </si>
-  <si>
-    <t>Indonesia</t>
-  </si>
-  <si>
-    <t>Jakarta Stock Exchange</t>
-  </si>
-  <si>
-    <t>.JK</t>
-  </si>
-  <si>
-    <t>Ireland</t>
-  </si>
-  <si>
-    <t>Irish Stock Exchange</t>
-  </si>
-  <si>
-    <t>.IR</t>
-  </si>
-  <si>
-    <t>Israel</t>
-  </si>
-  <si>
-    <t>Tel Aviv Stock Exchange</t>
-  </si>
-  <si>
-    <t>.TA</t>
-  </si>
-  <si>
-    <t>Italy</t>
-  </si>
-  <si>
-    <t>EuroTLX</t>
-  </si>
-  <si>
-    <t>.TI</t>
-  </si>
-  <si>
-    <t>Milan Stock Exchange</t>
-  </si>
-  <si>
-    <t>.MI</t>
-  </si>
-  <si>
-    <t>Japan</t>
-  </si>
-  <si>
-    <t>Nikkei Indices</t>
-  </si>
-  <si>
-    <t>Latvia</t>
-  </si>
-  <si>
-    <t>Nasdaq OMX Riga</t>
-  </si>
-  <si>
-    <t>.RG</t>
-  </si>
-  <si>
-    <t>Malaysia</t>
-  </si>
-  <si>
-    <t>Bursa Malaysia</t>
-  </si>
-  <si>
-    <t>.KL</t>
-  </si>
-  <si>
-    <t>Mexico</t>
-  </si>
-  <si>
-    <t>Mexico Stock Exchange</t>
-  </si>
-  <si>
-    <t>.MX</t>
-  </si>
-  <si>
-    <t>Netherlands</t>
-  </si>
-  <si>
-    <t>NYSE Euronext – Amsterdam</t>
-  </si>
-  <si>
-    <t>.AS</t>
-  </si>
-  <si>
-    <t>New Zealand</t>
-  </si>
-  <si>
-    <t>New Zealand Stock Exchange</t>
-  </si>
-  <si>
-    <t>.NZ</t>
-  </si>
-  <si>
-    <t>Norway</t>
-  </si>
-  <si>
-    <t>Oslo Stock Exchange</t>
-  </si>
-  <si>
-    <t>.OL</t>
-  </si>
-  <si>
-    <t>Portugal</t>
-  </si>
-  <si>
-    <t>NYSE Euronext – Lisbon</t>
-  </si>
-  <si>
-    <t>.LS</t>
-  </si>
-  <si>
-    <t>Qatar</t>
-  </si>
-  <si>
-    <t>Qatar Stock Exchange</t>
-  </si>
-  <si>
-    <t>.QA</t>
-  </si>
-  <si>
-    <t>Russia</t>
-  </si>
-  <si>
-    <t>Moscow Interbank Currency Exchange (MICEX)</t>
-  </si>
-  <si>
-    <t>.ME</t>
-  </si>
-  <si>
-    <t>Singapore</t>
-  </si>
-  <si>
-    <t>NKY</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AMS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RIX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ICX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EGX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SES</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>QSE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DUS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FRA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MUN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LSE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HAM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TWO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MAD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IOB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VIE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SHH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CBT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CME</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NBI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NYM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BUE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ASX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BRU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TOR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CVE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SGO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SHZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PRA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CPH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TLX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HEL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NXT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BRE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ATH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BSE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NSI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JKT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ISE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MIL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NZE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OSL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LIS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MCX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BAR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BIL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MFI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VAL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SWX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SET</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>STO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>KLS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MEX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SAO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BER</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PAR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TLV</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TLO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data Provider</t>
-  </si>
-  <si>
-    <t>United States of America</t>
-  </si>
-  <si>
-    <t>BATS Exchange</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Real-time</t>
-  </si>
-  <si>
-    <t>Direct from Exchange</t>
-  </si>
-  <si>
-    <t>Chicago Board of Trade</t>
-  </si>
-  <si>
-    <t>.CBT</t>
-  </si>
-  <si>
-    <t>10 min</t>
-  </si>
-  <si>
-    <t>Interactive Data Real-Time Services</t>
-  </si>
-  <si>
-    <t>Chicago Mercantile Exchange</t>
-  </si>
-  <si>
-    <t>.CME</t>
-  </si>
-  <si>
-    <t>Dow Jones Indexes</t>
-  </si>
-  <si>
-    <t>NASDAQ Stock Exchange</t>
-  </si>
-  <si>
-    <t>New York Board of Trade</t>
-  </si>
-  <si>
-    <t>.NYB</t>
-  </si>
-  <si>
-    <t>30 min</t>
-  </si>
-  <si>
-    <t>New York Mercantile Exchange</t>
-  </si>
-  <si>
-    <t>.NYM</t>
-  </si>
-  <si>
-    <t>New York Stock Exchange</t>
-  </si>
-  <si>
-    <t>Direct from Exchange***</t>
-  </si>
-  <si>
-    <t>OPRA</t>
-  </si>
-  <si>
-    <t>15 min</t>
-  </si>
-  <si>
-    <t>OTC Bulletin Board Market</t>
-  </si>
-  <si>
-    <t>OTC Markets Group</t>
-  </si>
-  <si>
-    <t>S &amp; P Indices</t>
-  </si>
-  <si>
-    <t>Argentina</t>
-  </si>
-  <si>
-    <t>Buenos Aires Stock Exchange</t>
-  </si>
-  <si>
-    <t>.BA</t>
-  </si>
-  <si>
-    <t>Austria</t>
-  </si>
-  <si>
-    <t>Vienna Stock Exchange</t>
-  </si>
-  <si>
-    <t>.VI</t>
-  </si>
-  <si>
-    <t>SIX Financial Information</t>
-  </si>
-  <si>
-    <t>Australia</t>
-  </si>
-  <si>
-    <t>Australian Stock Exchange</t>
-  </si>
-  <si>
-    <t>.AX</t>
-  </si>
-  <si>
-    <t>20 min</t>
-  </si>
-  <si>
-    <t>Belgium</t>
-  </si>
-  <si>
-    <t>NYSE Euronext - Brussels</t>
-  </si>
-  <si>
-    <t>.BR</t>
-  </si>
-  <si>
-    <t>Brazil</t>
-  </si>
-  <si>
-    <t>BOVESPA - Sao Paolo Stock Exchange</t>
-  </si>
-  <si>
-    <t>.SA</t>
-  </si>
-  <si>
-    <t>Canada</t>
   </si>
 </sst>
 </file>
@@ -1266,10 +1299,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1281,1518 +1314,1541 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>213</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>214</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>215</v>
       </c>
       <c r="D1" t="s">
-        <v>50</v>
+        <v>216</v>
       </c>
       <c r="E1" t="s">
-        <v>225</v>
+        <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>226</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>227</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>228</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>229</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>230</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>226</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>231</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>232</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>233</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>183</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>226</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>235</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>236</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>233</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>184</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>226</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>237</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>228</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>229</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>226</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>238</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>228</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>229</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>230</v>
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>226</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>239</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>240</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>241</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>185</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>226</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>242</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>243</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>241</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>186</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>226</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>244</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>228</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>229</v>
+        <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>245</v>
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>226</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>246</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>228</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>226</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>248</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>228</v>
+        <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>229</v>
+        <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>230</v>
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>226</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>249</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>228</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>238</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>226</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>250</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>228</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>229</v>
+        <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>251</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>252</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>253</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>241</v>
+        <v>17</v>
       </c>
       <c r="E14" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>187</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>254</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>255</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>256</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E15" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F15" t="s">
-        <v>181</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>258</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>259</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>260</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>261</v>
+        <v>37</v>
       </c>
       <c r="E16" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>188</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>262</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>263</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>264</v>
+        <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E17" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F17" t="s">
-        <v>189</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>265</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>266</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>267</v>
+        <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E18" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>220</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>268</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>220</v>
       </c>
       <c r="D19" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E19" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>190</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>268</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>221</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>222</v>
       </c>
       <c r="D20" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>191</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>223</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>224</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>225</v>
       </c>
       <c r="D21" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E21" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>192</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>226</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>227</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>228</v>
       </c>
       <c r="D22" t="s">
-        <v>241</v>
+        <v>17</v>
       </c>
       <c r="E22" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F22" t="s">
-        <v>182</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>226</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>229</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>230</v>
       </c>
       <c r="D23" t="s">
-        <v>241</v>
+        <v>17</v>
       </c>
       <c r="E23" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F23" t="s">
-        <v>193</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>231</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>232</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>233</v>
       </c>
       <c r="D24" t="s">
-        <v>261</v>
+        <v>37</v>
       </c>
       <c r="E24" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F24" t="s">
-        <v>194</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>234</v>
       </c>
       <c r="B25" t="s">
-        <v>69</v>
+        <v>235</v>
       </c>
       <c r="C25" t="s">
-        <v>70</v>
+        <v>236</v>
       </c>
       <c r="D25" t="s">
-        <v>229</v>
+        <v>5</v>
       </c>
       <c r="E25" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F25" t="s">
-        <v>195</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>71</v>
+        <v>237</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
+        <v>238</v>
       </c>
       <c r="C26" t="s">
-        <v>73</v>
+        <v>239</v>
       </c>
       <c r="D26" t="s">
-        <v>261</v>
+        <v>37</v>
       </c>
       <c r="E26" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F26" t="s">
-        <v>170</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>240</v>
       </c>
       <c r="B27" t="s">
-        <v>75</v>
+        <v>241</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>242</v>
       </c>
       <c r="D27" t="s">
-        <v>229</v>
+        <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F27" t="s">
-        <v>196</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>243</v>
       </c>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>244</v>
       </c>
       <c r="C28" t="s">
-        <v>79</v>
+        <v>245</v>
       </c>
       <c r="D28" t="s">
-        <v>229</v>
+        <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F28" t="s">
-        <v>197</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>80</v>
+        <v>246</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>247</v>
       </c>
       <c r="C29" t="s">
-        <v>82</v>
+        <v>248</v>
       </c>
       <c r="D29" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E29" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F29" t="s">
-        <v>198</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>246</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>249</v>
       </c>
       <c r="C30" t="s">
-        <v>84</v>
+        <v>250</v>
       </c>
       <c r="D30" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E30" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F30" t="s">
-        <v>222</v>
+        <v>166</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>251</v>
       </c>
       <c r="B31" t="s">
-        <v>86</v>
+        <v>252</v>
       </c>
       <c r="C31" t="s">
-        <v>87</v>
+        <v>253</v>
       </c>
       <c r="D31" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E31" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F31" t="s">
-        <v>221</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>85</v>
+        <v>251</v>
       </c>
       <c r="B32" t="s">
-        <v>88</v>
+        <v>254</v>
       </c>
       <c r="C32" t="s">
-        <v>89</v>
+        <v>255</v>
       </c>
       <c r="D32" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E32" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F32" t="s">
-        <v>199</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>85</v>
+        <v>251</v>
       </c>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>256</v>
       </c>
       <c r="C33" t="s">
-        <v>91</v>
+        <v>257</v>
       </c>
       <c r="D33" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E33" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F33" t="s">
-        <v>173</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>251</v>
       </c>
       <c r="B34" t="s">
-        <v>92</v>
+        <v>258</v>
       </c>
       <c r="C34" t="s">
-        <v>93</v>
+        <v>259</v>
       </c>
       <c r="D34" t="s">
-        <v>229</v>
+        <v>5</v>
       </c>
       <c r="E34" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F34" t="s">
-        <v>106</v>
+        <v>272</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>85</v>
+        <v>251</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>260</v>
       </c>
       <c r="C35" t="s">
-        <v>95</v>
+        <v>261</v>
       </c>
       <c r="D35" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E35" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F35" t="s">
-        <v>174</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>85</v>
+        <v>251</v>
       </c>
       <c r="B36" t="s">
-        <v>96</v>
+        <v>262</v>
       </c>
       <c r="C36" t="s">
-        <v>97</v>
+        <v>263</v>
       </c>
       <c r="D36" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E36" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F36" t="s">
-        <v>177</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>85</v>
+        <v>251</v>
       </c>
       <c r="B37" t="s">
-        <v>98</v>
+        <v>264</v>
       </c>
       <c r="C37" t="s">
-        <v>99</v>
+        <v>265</v>
       </c>
       <c r="D37" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E37" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F37" t="s">
-        <v>175</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>85</v>
+        <v>251</v>
       </c>
       <c r="B38" t="s">
-        <v>100</v>
+        <v>266</v>
       </c>
       <c r="C38" t="s">
-        <v>101</v>
+        <v>267</v>
       </c>
       <c r="D38" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E38" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F38" t="s">
-        <v>107</v>
+        <v>273</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>85</v>
+        <v>251</v>
       </c>
       <c r="B39" t="s">
-        <v>102</v>
+        <v>268</v>
       </c>
       <c r="C39" t="s">
-        <v>103</v>
+        <v>269</v>
       </c>
       <c r="D39" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E39" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F39" t="s">
-        <v>106</v>
+        <v>272</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>104</v>
+        <v>270</v>
       </c>
       <c r="B40" t="s">
-        <v>108</v>
+        <v>274</v>
       </c>
       <c r="C40" t="s">
-        <v>109</v>
+        <v>275</v>
       </c>
       <c r="D40" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E40" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F40" t="s">
-        <v>200</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>110</v>
+        <v>276</v>
       </c>
       <c r="B41" t="s">
-        <v>111</v>
+        <v>58</v>
       </c>
       <c r="C41" t="s">
-        <v>112</v>
+        <v>59</v>
       </c>
       <c r="D41" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E41" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F41" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>113</v>
+        <v>60</v>
       </c>
       <c r="B42" t="s">
-        <v>114</v>
+        <v>61</v>
       </c>
       <c r="C42" t="s">
-        <v>115</v>
+        <v>62</v>
       </c>
       <c r="D42" t="s">
-        <v>229</v>
+        <v>5</v>
       </c>
       <c r="E42" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F42" t="s">
-        <v>169</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>116</v>
+        <v>63</v>
       </c>
       <c r="B43" t="s">
-        <v>117</v>
+        <v>64</v>
       </c>
       <c r="C43" t="s">
-        <v>118</v>
+        <v>65</v>
       </c>
       <c r="D43" t="s">
-        <v>229</v>
+        <v>5</v>
       </c>
       <c r="E43" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F43" t="s">
-        <v>201</v>
+        <v>147</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>116</v>
+        <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>119</v>
+        <v>66</v>
       </c>
       <c r="C44" t="s">
-        <v>120</v>
+        <v>67</v>
       </c>
       <c r="D44" t="s">
-        <v>121</v>
+        <v>68</v>
       </c>
       <c r="E44" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F44" t="s">
-        <v>202</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>122</v>
+        <v>69</v>
       </c>
       <c r="B45" t="s">
-        <v>123</v>
+        <v>70</v>
       </c>
       <c r="C45" t="s">
-        <v>124</v>
+        <v>71</v>
       </c>
       <c r="D45" t="s">
-        <v>233</v>
+        <v>9</v>
       </c>
       <c r="E45" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F45" t="s">
-        <v>203</v>
+        <v>148</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>125</v>
+        <v>72</v>
       </c>
       <c r="B46" t="s">
-        <v>126</v>
+        <v>73</v>
       </c>
       <c r="C46" t="s">
-        <v>127</v>
+        <v>74</v>
       </c>
       <c r="D46" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E46" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F46" t="s">
-        <v>204</v>
+        <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>128</v>
+        <v>75</v>
       </c>
       <c r="B47" t="s">
-        <v>129</v>
+        <v>76</v>
       </c>
       <c r="C47" t="s">
-        <v>130</v>
+        <v>77</v>
       </c>
       <c r="D47" t="s">
-        <v>261</v>
+        <v>37</v>
       </c>
       <c r="E47" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F47" t="s">
-        <v>223</v>
+        <v>167</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>131</v>
+        <v>78</v>
       </c>
       <c r="B48" t="s">
-        <v>132</v>
+        <v>79</v>
       </c>
       <c r="C48" t="s">
-        <v>133</v>
+        <v>80</v>
       </c>
       <c r="D48" t="s">
-        <v>261</v>
+        <v>37</v>
       </c>
       <c r="E48" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F48" t="s">
-        <v>224</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>131</v>
+        <v>78</v>
       </c>
       <c r="B49" t="s">
-        <v>134</v>
+        <v>81</v>
       </c>
       <c r="C49" t="s">
-        <v>135</v>
+        <v>82</v>
       </c>
       <c r="D49" t="s">
-        <v>261</v>
+        <v>37</v>
       </c>
       <c r="E49" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F49" t="s">
-        <v>205</v>
+        <v>150</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>136</v>
+        <v>83</v>
       </c>
       <c r="B50" t="s">
-        <v>137</v>
+        <v>84</v>
       </c>
       <c r="C50" t="s">
-        <v>228</v>
+        <v>4</v>
       </c>
       <c r="D50" t="s">
-        <v>241</v>
+        <v>17</v>
       </c>
       <c r="E50" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F50" t="s">
-        <v>166</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>138</v>
+        <v>85</v>
       </c>
       <c r="B51" t="s">
-        <v>139</v>
+        <v>86</v>
       </c>
       <c r="C51" t="s">
-        <v>140</v>
+        <v>87</v>
       </c>
       <c r="D51" t="s">
-        <v>229</v>
+        <v>5</v>
       </c>
       <c r="E51" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F51" t="s">
-        <v>168</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>141</v>
+        <v>88</v>
       </c>
       <c r="B52" t="s">
-        <v>142</v>
+        <v>89</v>
       </c>
       <c r="C52" t="s">
-        <v>143</v>
+        <v>90</v>
       </c>
       <c r="D52" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E52" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F52" t="s">
-        <v>218</v>
+        <v>162</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>144</v>
+        <v>91</v>
       </c>
       <c r="B53" t="s">
-        <v>145</v>
+        <v>92</v>
       </c>
       <c r="C53" t="s">
-        <v>146</v>
+        <v>93</v>
       </c>
       <c r="D53" t="s">
-        <v>261</v>
+        <v>37</v>
       </c>
       <c r="E53" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F53" t="s">
-        <v>219</v>
+        <v>163</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>147</v>
+        <v>94</v>
       </c>
       <c r="B54" t="s">
-        <v>148</v>
+        <v>95</v>
       </c>
       <c r="C54" t="s">
-        <v>149</v>
+        <v>96</v>
       </c>
       <c r="D54" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E54" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F54" t="s">
-        <v>167</v>
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>150</v>
+        <v>97</v>
       </c>
       <c r="B55" t="s">
-        <v>151</v>
+        <v>98</v>
       </c>
       <c r="C55" t="s">
-        <v>152</v>
+        <v>99</v>
       </c>
       <c r="D55" t="s">
-        <v>261</v>
+        <v>37</v>
       </c>
       <c r="E55" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F55" t="s">
-        <v>206</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>153</v>
+        <v>100</v>
       </c>
       <c r="B56" t="s">
-        <v>154</v>
+        <v>101</v>
       </c>
       <c r="C56" t="s">
-        <v>155</v>
+        <v>102</v>
       </c>
       <c r="D56" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E56" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F56" t="s">
-        <v>207</v>
+        <v>151</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>156</v>
+        <v>103</v>
       </c>
       <c r="B57" t="s">
-        <v>157</v>
+        <v>104</v>
       </c>
       <c r="C57" t="s">
-        <v>158</v>
+        <v>105</v>
       </c>
       <c r="D57" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E57" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F57" t="s">
-        <v>208</v>
+        <v>152</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>159</v>
+        <v>106</v>
       </c>
       <c r="B58" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="C58" t="s">
-        <v>161</v>
+        <v>108</v>
       </c>
       <c r="D58" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E58" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F58" t="s">
-        <v>172</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>162</v>
+        <v>109</v>
       </c>
       <c r="B59" t="s">
-        <v>163</v>
+        <v>110</v>
       </c>
       <c r="C59" t="s">
-        <v>164</v>
+        <v>111</v>
       </c>
       <c r="D59" t="s">
-        <v>229</v>
+        <v>5</v>
       </c>
       <c r="E59" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F59" t="s">
-        <v>209</v>
+        <v>153</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>165</v>
+        <v>112</v>
       </c>
       <c r="B60" t="s">
-        <v>0</v>
+        <v>168</v>
       </c>
       <c r="C60" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="D60" t="s">
-        <v>261</v>
+        <v>37</v>
       </c>
       <c r="E60" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F60" t="s">
-        <v>171</v>
+        <v>118</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>2</v>
+        <v>170</v>
       </c>
       <c r="B61" t="s">
-        <v>3</v>
+        <v>171</v>
       </c>
       <c r="C61" t="s">
-        <v>4</v>
+        <v>172</v>
       </c>
       <c r="D61" t="s">
-        <v>261</v>
+        <v>37</v>
       </c>
       <c r="E61" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F61" t="s">
-        <v>45</v>
+        <v>211</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>2</v>
+        <v>170</v>
       </c>
       <c r="B62" t="s">
-        <v>5</v>
+        <v>173</v>
       </c>
       <c r="C62" t="s">
-        <v>6</v>
+        <v>174</v>
       </c>
       <c r="D62" t="s">
-        <v>261</v>
+        <v>37</v>
       </c>
       <c r="E62" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F62" t="s">
-        <v>46</v>
+        <v>212</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>7</v>
+        <v>175</v>
       </c>
       <c r="B63" t="s">
-        <v>8</v>
+        <v>176</v>
       </c>
       <c r="C63" t="s">
-        <v>9</v>
+        <v>177</v>
       </c>
       <c r="D63" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E63" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F63" t="s">
-        <v>210</v>
+        <v>154</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>7</v>
+        <v>175</v>
       </c>
       <c r="B64" t="s">
-        <v>10</v>
+        <v>178</v>
       </c>
       <c r="C64" t="s">
-        <v>11</v>
+        <v>179</v>
       </c>
       <c r="D64" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E64" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F64" t="s">
-        <v>211</v>
+        <v>155</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>7</v>
+        <v>175</v>
       </c>
       <c r="B65" t="s">
-        <v>12</v>
+        <v>180</v>
       </c>
       <c r="C65" t="s">
-        <v>13</v>
+        <v>181</v>
       </c>
       <c r="D65" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E65" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F65" t="s">
-        <v>212</v>
+        <v>156</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>7</v>
+        <v>175</v>
       </c>
       <c r="B66" t="s">
-        <v>14</v>
+        <v>182</v>
       </c>
       <c r="C66" t="s">
-        <v>15</v>
+        <v>183</v>
       </c>
       <c r="D66" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E66" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F66" t="s">
-        <v>179</v>
+        <v>126</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>7</v>
+        <v>175</v>
       </c>
       <c r="B67" t="s">
-        <v>16</v>
+        <v>184</v>
       </c>
       <c r="C67" t="s">
-        <v>17</v>
+        <v>185</v>
       </c>
       <c r="D67" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E67" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F67" t="s">
-        <v>213</v>
+        <v>157</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>18</v>
+        <v>186</v>
       </c>
       <c r="B68" t="s">
-        <v>19</v>
+        <v>187</v>
       </c>
       <c r="C68" t="s">
-        <v>20</v>
+        <v>188</v>
       </c>
       <c r="D68" t="s">
-        <v>229</v>
+        <v>5</v>
       </c>
       <c r="E68" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F68" t="s">
-        <v>217</v>
+        <v>161</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>21</v>
+        <v>189</v>
       </c>
       <c r="B69" t="s">
-        <v>22</v>
+        <v>190</v>
       </c>
       <c r="C69" t="s">
-        <v>23</v>
+        <v>191</v>
       </c>
       <c r="D69" t="s">
-        <v>241</v>
+        <v>17</v>
       </c>
       <c r="E69" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F69" t="s">
-        <v>214</v>
+        <v>158</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>24</v>
+        <v>192</v>
       </c>
       <c r="B70" t="s">
-        <v>25</v>
+        <v>193</v>
       </c>
       <c r="C70" t="s">
-        <v>26</v>
+        <v>194</v>
       </c>
       <c r="D70" t="s">
-        <v>261</v>
+        <v>37</v>
       </c>
       <c r="E70" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F70" t="s">
-        <v>178</v>
+        <v>125</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>24</v>
+        <v>192</v>
       </c>
       <c r="B71" t="s">
-        <v>27</v>
+        <v>195</v>
       </c>
       <c r="C71" t="s">
-        <v>28</v>
+        <v>196</v>
       </c>
       <c r="D71" t="s">
-        <v>261</v>
+        <v>37</v>
       </c>
       <c r="E71" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F71" t="s">
-        <v>105</v>
+        <v>271</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>29</v>
+        <v>197</v>
       </c>
       <c r="B72" t="s">
-        <v>30</v>
+        <v>198</v>
       </c>
       <c r="C72" t="s">
-        <v>31</v>
+        <v>199</v>
       </c>
       <c r="D72" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E72" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F72" t="s">
-        <v>215</v>
+        <v>159</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>32</v>
+        <v>200</v>
       </c>
       <c r="B73" t="s">
-        <v>33</v>
+        <v>201</v>
       </c>
       <c r="C73" t="s">
-        <v>34</v>
+        <v>202</v>
       </c>
       <c r="D73" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E73" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F73" t="s">
-        <v>51</v>
+        <v>217</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>35</v>
+        <v>203</v>
       </c>
       <c r="B74" t="s">
-        <v>36</v>
+        <v>204</v>
       </c>
       <c r="C74" t="s">
-        <v>228</v>
+        <v>4</v>
       </c>
       <c r="D74" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E74" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F74" t="s">
-        <v>52</v>
+        <v>218</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>35</v>
+        <v>203</v>
       </c>
       <c r="B75" t="s">
+        <v>48</v>
+      </c>
+      <c r="C75" t="s">
+        <v>205</v>
+      </c>
+      <c r="D75" t="s">
         <v>37</v>
       </c>
-      <c r="C75" t="s">
-        <v>38</v>
-      </c>
-      <c r="D75" t="s">
-        <v>261</v>
-      </c>
       <c r="E75" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F75" t="s">
-        <v>176</v>
+        <v>123</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>35</v>
+        <v>203</v>
       </c>
       <c r="B76" t="s">
+        <v>49</v>
+      </c>
+      <c r="C76" t="s">
+        <v>206</v>
+      </c>
+      <c r="D76" t="s">
         <v>37</v>
       </c>
-      <c r="C76" t="s">
-        <v>39</v>
-      </c>
-      <c r="D76" t="s">
-        <v>261</v>
-      </c>
       <c r="E76" t="s">
-        <v>257</v>
+        <v>33</v>
       </c>
       <c r="F76" t="s">
-        <v>180</v>
+        <v>127</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>40</v>
+        <v>207</v>
       </c>
       <c r="B77" t="s">
-        <v>41</v>
+        <v>208</v>
       </c>
       <c r="C77" t="s">
-        <v>42</v>
+        <v>209</v>
       </c>
       <c r="D77" t="s">
-        <v>247</v>
+        <v>23</v>
       </c>
       <c r="E77" t="s">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F77" t="s">
-        <v>216</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" t="s">
+        <v>56</v>
+      </c>
+      <c r="B78" t="s">
+        <v>53</v>
+      </c>
+      <c r="C78" t="s">
+        <v>55</v>
+      </c>
+      <c r="F78" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>